<commit_message>
major upgrade to plumbing data
- abandoned camelCase for table names
- plumBrand table is now just brand
- errors in price data fixed

-this commit before making fitting price input
</commit_message>
<xml_diff>
--- a/backend/data/plumData/plumTableData/plumPrice.xlsx
+++ b/backend/data/plumData/plumTableData/plumPrice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\MY_PROJECTS\web_application\backend\data\plumData\plumTableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7605422E-9911-4195-8AA9-2CB7743AEC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511194E6-FDE6-4CB2-BA3F-38149ECDE578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{A0BBE691-86F4-4964-8F22-F4C94C854054}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{A0BBE691-86F4-4964-8F22-F4C94C854054}"/>
   </bookViews>
   <sheets>
     <sheet name="size" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="197">
   <si>
     <t>20mm</t>
   </si>
@@ -1098,8 +1098,8 @@
         <v>("20mm", "1/2\"")</v>
       </c>
       <c r="H2" t="str" cm="1">
-        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES",(TRANSPOSE(G2:G34)&amp;","))</f>
-        <v>INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES("20mm", "1/2\""),("25mm", "3/4\""),("32mm", "1\""),("40mm", "1 1/4\""),("50mm", "1 1/2\""),("63mm", "2\""),("75mm", "2 1/2\""),("90mm", "3\""),("110mm", "4\""),("25mm x 20mm", "3/4\" x 1/2\""),("32mm x 20mm", "1\" x 1/2\""),("32mm x 25mm", "1\" x 3/4\""),("40mm x 20mm", "1 1/4\" x 1/2\""),("40mm x 25mm", "1 1/4\" x 3/4\""),("40mm x 32mm", "1 1/4\" x 1\""),("50mmx 20mm", "1 1/2\" x 1/2\""),("50mm x 25mm", "1 1/2\" x 3/4\""),("50mm x 32mm", "1 1/2\" x 1\""),("50mm x 40mm", "1 1/2\" x 1 1/4\""),("63mm x 20mm", "2\" x 1/2\""),("63mm x 25mm", "2\" x 3/4\""),("63mm x 32mm", "2\" x 1\""),("63mm x 40mm", "2\" x 1 1/4\""),("63mm x 50mm", "2\" x 1 1/2\""),("90mm x 40mm", "3\" x 1 1/4\""),("90mm x 50mm", "3\" x 1 1/2\""),("90mm x 63mm", "3\" x 2\""),("90mm x 75mm", "3\" x 2 1/2\""),("110mm x 50mm", "4\" x 1 1/2\""),("110mm x 63mm", "4\" x 2\""),("110mm x 75mm", "4\" x 2 1/2\""),("110mm x 90mm", "4\" x 3\""),("160mm", "6\""),</v>
+        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plum_size (plum_size_imperial,plum_size_metric) VALUES",(TRANSPOSE(G2:G34)&amp;","))</f>
+        <v>INSERT INTO plum_size (plum_size_imperial,plum_size_metric) VALUES("20mm", "1/2\""),("25mm", "3/4\""),("32mm", "1\""),("40mm", "1 1/4\""),("50mm", "1 1/2\""),("63mm", "2\""),("75mm", "2 1/2\""),("90mm", "3\""),("110mm", "4\""),("25mm x 20mm", "3/4\" x 1/2\""),("32mm x 20mm", "1\" x 1/2\""),("32mm x 25mm", "1\" x 3/4\""),("40mm x 20mm", "1 1/4\" x 1/2\""),("40mm x 25mm", "1 1/4\" x 3/4\""),("40mm x 32mm", "1 1/4\" x 1\""),("50mmx 20mm", "1 1/2\" x 1/2\""),("50mm x 25mm", "1 1/2\" x 3/4\""),("50mm x 32mm", "1 1/2\" x 1\""),("50mm x 40mm", "1 1/2\" x 1 1/4\""),("63mm x 20mm", "2\" x 1/2\""),("63mm x 25mm", "2\" x 3/4\""),("63mm x 32mm", "2\" x 1\""),("63mm x 40mm", "2\" x 1 1/4\""),("63mm x 50mm", "2\" x 1 1/2\""),("90mm x 40mm", "3\" x 1 1/4\""),("90mm x 50mm", "3\" x 1 1/2\""),("90mm x 63mm", "3\" x 2\""),("90mm x 75mm", "3\" x 2 1/2\""),("110mm x 50mm", "4\" x 1 1/2\""),("110mm x 63mm", "4\" x 2\""),("110mm x 75mm", "4\" x 2 1/2\""),("110mm x 90mm", "4\" x 3\""),("160mm", "6\""),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1943,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEDC410-2645-479E-B85E-F5D25DF089AA}">
   <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="L192" sqref="L192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6950,8 +6950,8 @@
         <v>(1, 1, 2, 1, 2)</v>
       </c>
       <c r="H2" t="str" cm="1">
-        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES",(TRANSPOSE(G2:G176)&amp;","))</f>
-        <v>INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES(1, 1, 2, 1, 2),(1, 1, 4, 2, 2),(1, 1, 4, 3, 2),(1, 1, 4, 4, 2),(1, 1, 4, 5, 2),(1, 1, 4, 6, 2),(1, 1, 4, 7, 2),(1, 1, 4, 8, 2),(1, 1, 4, 9, 2),(2, 1, 2, 1, 2),(2, 1, 4, 2, 2),(2, 1, 4, 3, 2),(2, 1, 4, 4, 2),(2, 1, 4, 5, 2),(2, 1, 4, 6, 2),(2, 1, 4, 7, 2),(2, 1, 4, 8, 2),(2, 1, 4, 9, 2),(3, 1, 2, 1, 2),(3, 1, 4, 2, 2),(3, 1, 4, 3, 2),(3, 1, 4, 4, 2),(3, 1, 4, 5, 2),(3, 1, 4, 6, 2),(3, 1, 4, 7, 2),(3, 1, 4, 8, 2),(3, 1, 4, 9, 2),(4, 1, 2, 1, 2),(4, 1, 4, 2, 2),(4, 1, 4, 3, 2),(4, 1, 4, 4, 2),(4, 1, 4, 5, 2),(4, 1, 4, 6, 2),(4, 1, 4, 7, 2),(4, 1, 4, 8, 2),(4, 1, 4, 9, 2),(5, 1, 2, 1, 2),(5, 1, 4, 2, 2),(5, 1, 4, 3, 2),(5, 1, 4, 4, 2),(5, 1, 4, 5, 2),(5, 1, 4, 6, 2),(5, 1, 4, 7, 2),(5, 1, 4, 8, 2),(5, 1, 4, 9, 2),(6, 1, 2, 1, 2),(6, 1, 4, 2, 2),(6, 1, 4, 3, 2),(6, 1, 4, 4, 2),(6, 1, 4, 5, 2),(6, 1, 4, 6, 2),(6, 1, 4, 7, 2),(6, 1, 4, 8, 2),(6, 1, 4, 9, 2),(7, 1, 2, 1, 2),(7, 1, 4, 2, 2),(7, 1, 4, 3, 2),(7, 1, 4, 4, 2),(7, 1, 4, 5, 2),(7, 1, 4, 6, 2),(7, 1, 4, 7, 2),(7, 1, 4, 8, 2),(7, 1, 4, 9, 2),(8, 1, 2, 1, 2),(8, 1, 4, 2, 2),(8, 1, 4, 3, 2),(8, 1, 4, 4, 2),(8, 1, 4, 5, 2),(8, 1, 4, 6, 2),(8, 1, 4, 7, 2),(8, 1, 4, 8, 2),(8, 1, 4, 9, 2),(9, 1, 2, 1, 2),(9, 1, 4, 2, 2),(9, 1, 4, 3, 2),(9, 1, 4, 4, 2),(9, 1, 4, 5, 2),(9, 1, 4, 6, 2),(10, 1, 4, 10, 2),(10, 1, 4, 11, 2),(10, 1, 4, 12, 2),(10, 1, 4, 13, 2),(10, 1, 4, 14, 2),(10, 1, 4, 15, 2),(10, 1, 4, 16, 2),(10, 1, 4, 17, 2),(10, 1, 4, 18, 2),(10, 1, 4, 19, 2),(10, 1, 4, 20, 2),(10, 1, 4, 21, 2),(10, 1, 4, 22, 2),(10, 1, 4, 23, 2),(10, 1, 4, 24, 2),(10, 1, 4, 25, 2),(10, 1, 4, 26, 2),(10, 1, 4, 27, 2),(10, 1, 4, 28, 2),(10, 1, 4, 29, 2),(10, 1, 4, 30, 2),(10, 1, 4, 31, 2),(10, 1, 4, 32, 2),(11, 1, 4, 10, 2),(11, 1, 4, 11, 2),(11, 1, 4, 12, 2),(11, 1, 4, 13, 2),(11, 1, 4, 14, 2),(11, 1, 4, 15, 2),(11, 1, 4, 16, 2),(11, 1, 4, 17, 2),(11, 1, 4, 18, 2),(11, 1, 4, 19, 2),(11, 1, 4, 20, 2),(11, 1, 4, 21, 2),(11, 1, 4, 22, 2),(11, 1, 4, 23, 2),(11, 1, 4, 24, 2),(11, 1, 4, 25, 2),(11, 1, 4, 26, 2),(11, 1, 4, 27, 2),(11, 1, 4, 28, 2),(11, 1, 4, 29, 2),(11, 1, 4, 30, 2),(11, 1, 4, 31, 2),(11, 1, 4, 32, 2),(12, 1, 4, 10, 2),(13, 1, 4, 11, 2),(14, 1, 2, 1, 2),(15, 1, 2, 1, 2),(16, 1, 2, 1, 2),(17, 1, 2, 1, 2),(18, 1, 2, 1, 2),(19, 1, 5, 10, 2),(19, 1, 5, 11, 2),(20, 1, 5, 10, 2),(21, 1, 2, 1, 2),(21, 1, 4, 2, 2),(21, 1, 4, 3, 2),(9, 1, 9, 4, 4),(9, 1, 9, 5, 4),(9, 1, 9, 6, 4),(9, 1, 9, 9, 4),(6, 1, 9, 4, 4),(6, 1, 9, 5, 4),(6, 1, 9, 6, 4),(6, 1, 9, 9, 4),(5, 1, 9, 4, 4),(5, 1, 9, 5, 4),(5, 1, 9, 6, 4),(5, 1, 9, 9, 4),(22, 1, 9, 4, 4),(22, 1, 9, 5, 4),(22, 1, 9, 9, 4),(23, 1, 9, 4, 4),(23, 1, 9, 5, 4),(23, 1, 9, 6, 4),(23, 1, 9, 9, 4),(24, 1, 9, 4, 4),(24, 1, 9, 5, 4),(24, 1, 9, 6, 4),(24, 1, 9, 9, 4),(25, 1, 9, 4, 4),(25, 1, 9, 5, 4),(25, 1, 9, 6, 4),(25, 1, 9, 9, 4),(26, 1, 9, 4, 4),(26, 1, 9, 5, 4),(26, 1, 9, 6, 4),(26, 1, 9, 9, 4),(27, 1, 9, 4, 4),(27, 1, 9, 5, 4),(27, 1, 9, 9, 4),(28, 1, 9, 4, 4),(28, 1, 9, 5, 4),(28, 1, 9, 6, 4),(28, 1, 9, 9, 4),</v>
+        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plum_fitting_info (plum_fitting_id,plum_grade_id,plum_size_id,plum_type_id) VALUES",(TRANSPOSE(G2:G176)&amp;","))</f>
+        <v>INSERT INTO plum_fitting_info (plum_fitting_id,plum_grade_id,plum_size_id,plum_type_id) VALUES(1, 1, 2, 1, 2),(1, 1, 4, 2, 2),(1, 1, 4, 3, 2),(1, 1, 4, 4, 2),(1, 1, 4, 5, 2),(1, 1, 4, 6, 2),(1, 1, 4, 7, 2),(1, 1, 4, 8, 2),(1, 1, 4, 9, 2),(2, 1, 2, 1, 2),(2, 1, 4, 2, 2),(2, 1, 4, 3, 2),(2, 1, 4, 4, 2),(2, 1, 4, 5, 2),(2, 1, 4, 6, 2),(2, 1, 4, 7, 2),(2, 1, 4, 8, 2),(2, 1, 4, 9, 2),(3, 1, 2, 1, 2),(3, 1, 4, 2, 2),(3, 1, 4, 3, 2),(3, 1, 4, 4, 2),(3, 1, 4, 5, 2),(3, 1, 4, 6, 2),(3, 1, 4, 7, 2),(3, 1, 4, 8, 2),(3, 1, 4, 9, 2),(4, 1, 2, 1, 2),(4, 1, 4, 2, 2),(4, 1, 4, 3, 2),(4, 1, 4, 4, 2),(4, 1, 4, 5, 2),(4, 1, 4, 6, 2),(4, 1, 4, 7, 2),(4, 1, 4, 8, 2),(4, 1, 4, 9, 2),(5, 1, 2, 1, 2),(5, 1, 4, 2, 2),(5, 1, 4, 3, 2),(5, 1, 4, 4, 2),(5, 1, 4, 5, 2),(5, 1, 4, 6, 2),(5, 1, 4, 7, 2),(5, 1, 4, 8, 2),(5, 1, 4, 9, 2),(6, 1, 2, 1, 2),(6, 1, 4, 2, 2),(6, 1, 4, 3, 2),(6, 1, 4, 4, 2),(6, 1, 4, 5, 2),(6, 1, 4, 6, 2),(6, 1, 4, 7, 2),(6, 1, 4, 8, 2),(6, 1, 4, 9, 2),(7, 1, 2, 1, 2),(7, 1, 4, 2, 2),(7, 1, 4, 3, 2),(7, 1, 4, 4, 2),(7, 1, 4, 5, 2),(7, 1, 4, 6, 2),(7, 1, 4, 7, 2),(7, 1, 4, 8, 2),(7, 1, 4, 9, 2),(8, 1, 2, 1, 2),(8, 1, 4, 2, 2),(8, 1, 4, 3, 2),(8, 1, 4, 4, 2),(8, 1, 4, 5, 2),(8, 1, 4, 6, 2),(8, 1, 4, 7, 2),(8, 1, 4, 8, 2),(8, 1, 4, 9, 2),(9, 1, 2, 1, 2),(9, 1, 4, 2, 2),(9, 1, 4, 3, 2),(9, 1, 4, 4, 2),(9, 1, 4, 5, 2),(9, 1, 4, 6, 2),(10, 1, 4, 10, 2),(10, 1, 4, 11, 2),(10, 1, 4, 12, 2),(10, 1, 4, 13, 2),(10, 1, 4, 14, 2),(10, 1, 4, 15, 2),(10, 1, 4, 16, 2),(10, 1, 4, 17, 2),(10, 1, 4, 18, 2),(10, 1, 4, 19, 2),(10, 1, 4, 20, 2),(10, 1, 4, 21, 2),(10, 1, 4, 22, 2),(10, 1, 4, 23, 2),(10, 1, 4, 24, 2),(10, 1, 4, 25, 2),(10, 1, 4, 26, 2),(10, 1, 4, 27, 2),(10, 1, 4, 28, 2),(10, 1, 4, 29, 2),(10, 1, 4, 30, 2),(10, 1, 4, 31, 2),(10, 1, 4, 32, 2),(11, 1, 4, 10, 2),(11, 1, 4, 11, 2),(11, 1, 4, 12, 2),(11, 1, 4, 13, 2),(11, 1, 4, 14, 2),(11, 1, 4, 15, 2),(11, 1, 4, 16, 2),(11, 1, 4, 17, 2),(11, 1, 4, 18, 2),(11, 1, 4, 19, 2),(11, 1, 4, 20, 2),(11, 1, 4, 21, 2),(11, 1, 4, 22, 2),(11, 1, 4, 23, 2),(11, 1, 4, 24, 2),(11, 1, 4, 25, 2),(11, 1, 4, 26, 2),(11, 1, 4, 27, 2),(11, 1, 4, 28, 2),(11, 1, 4, 29, 2),(11, 1, 4, 30, 2),(11, 1, 4, 31, 2),(11, 1, 4, 32, 2),(12, 1, 4, 10, 2),(13, 1, 4, 11, 2),(14, 1, 2, 1, 2),(15, 1, 2, 1, 2),(16, 1, 2, 1, 2),(17, 1, 2, 1, 2),(18, 1, 2, 1, 2),(19, 1, 5, 10, 2),(19, 1, 5, 11, 2),(20, 1, 5, 10, 2),(21, 1, 2, 1, 2),(21, 1, 4, 2, 2),(21, 1, 4, 3, 2),(9, 1, 9, 4, 4),(9, 1, 9, 5, 4),(9, 1, 9, 6, 4),(9, 1, 9, 9, 4),(6, 1, 9, 4, 4),(6, 1, 9, 5, 4),(6, 1, 9, 6, 4),(6, 1, 9, 9, 4),(5, 1, 9, 4, 4),(5, 1, 9, 5, 4),(5, 1, 9, 6, 4),(5, 1, 9, 9, 4),(22, 1, 9, 4, 4),(22, 1, 9, 5, 4),(22, 1, 9, 9, 4),(23, 1, 9, 4, 4),(23, 1, 9, 5, 4),(23, 1, 9, 6, 4),(23, 1, 9, 9, 4),(24, 1, 9, 4, 4),(24, 1, 9, 5, 4),(24, 1, 9, 6, 4),(24, 1, 9, 9, 4),(25, 1, 9, 4, 4),(25, 1, 9, 5, 4),(25, 1, 9, 6, 4),(25, 1, 9, 9, 4),(26, 1, 9, 4, 4),(26, 1, 9, 5, 4),(26, 1, 9, 6, 4),(26, 1, 9, 9, 4),(27, 1, 9, 4, 4),(27, 1, 9, 5, 4),(27, 1, 9, 9, 4),(28, 1, 9, 4, 4),(28, 1, 9, 5, 4),(28, 1, 9, 6, 4),(28, 1, 9, 9, 4),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -11201,25 +11201,24 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD72405-4BAA-4BE0-9E9A-35EF3BE8961C}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -11230,22 +11229,19 @@
         <v>176</v>
       </c>
       <c r="D1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="E1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11262,25 +11258,22 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <f>G2*3.28</f>
+        <f>F2*3.28</f>
         <v>13.12</v>
       </c>
-      <c r="I2" t="str">
-        <f>_xlfn.CONCAT( "(",B2,", ", C2,", ", D2,", ", E2,", ", F2,", ", G2,", ", H2,")")</f>
-        <v>(1, 1, 1, 1, 1, 4, 13.12)</v>
-      </c>
-      <c r="J2" t="str" cm="1">
-        <f t="array" ref="J2">_xlfn.CONCAT("INSERT INTO plumpipeinfos (plumGradeId,plumSizeId,plumBrandId,plumPipeTypeId,plumPipeEndType,PlumPipeLengthMetric,plumPipeLengthImperial) VALUES",(TRANSPOSE(I2:I32)&amp;","))</f>
-        <v>INSERT INTO plumpipeinfos (plumGradeId,plumSizeId,plumBrandId,plumPipeTypeId,plumPipeEndType,PlumPipeLengthMetric,plumPipeLengthImperial) VALUES(1, 1, 1, 1, 1, 4, 13.12),(3, 2, 1, 1, 1, 4, 13.12),(3, 3, 1, 1, 1, 4, 13.12),(3, 4, 1, 1, 1, 4, 13.12),(3, 5, 1, 1, 1, 4, 13.12),(3, 6, 1, 1, 1, 4, 13.12),(3, 7, 1, 1, 1, 4, 13.12),(3, 8, 1, 1, 1, 4, 13.12),(3, 9, 1, 1, 1, 6, 19.68),(6, 2, 1, 1, 1, 4, 13.12),(6, 3, 1, 1, 1, 4, 13.12),(6, 4, 1, 1, 1, 4, 13.12),(6, 5, 1, 1, 1, 4, 13.12),(6, 6, 1, 1, 1, 4, 13.12),(6, 7, 1, 1, 1, 4, 13.12),(6, 8, 1, 1, 1, 4, 13.12),(6, 9, 1, 1, 1, 6, 19.68),(7, 5, 1, 2, 1, 4, 13.12),(7, 6, 1, 2, 1, 4, 13.12),(7, 7, 1, 2, 1, 4, 13.12),(7, 8, 1, 2, 1, 4, 13.12),(7, 9, 1, 2, 1, 6, 19.68),(7, 33, 1, 2, 1, 6, 19.68),(8, 9, 1, 2, 2, 6, 19.68),(8, 33, 1, 2, 2, 6, 19.68),(7, 5, 1, 2, 2, 4, 13.12),(7, 6, 1, 2, 2, 4, 13.12),(7, 7, 1, 2, 2, 4, 13.12),(7, 8, 1, 2, 2, 4, 13.12),(7, 9, 1, 2, 2, 6, 19.68),(7, 33, 1, 2, 2, 6, 19.68),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT( "(",B2,",", C2,",", D2,",", E2,",", F2,",", G2,")")</f>
+        <v>(1,1,1,1,4,13.12)</v>
+      </c>
+      <c r="I2" t="str" cm="1">
+        <f t="array" ref="I2">_xlfn.CONCAT("INSERT INTO plum_pipe_info (plum_grade_id,plum_size_id,plum_brand_id,plum_pipe_type_id,plum_pipe_end_type,plum_pipe_length_metric,plum_pipe_length_imperial) VALUES",(TRANSPOSE(H2:H32)&amp;","))</f>
+        <v>INSERT INTO plum_pipe_info (plum_grade_id,plum_size_id,plum_brand_id,plum_pipe_type_id,plum_pipe_end_type,plum_pipe_length_metric,plum_pipe_length_imperial) VALUES(1,1,1,1,4,13.12),(3,2,1,1,4,13.12),(3,3,1,1,4,13.12),(3,4,1,1,4,13.12),(3,5,1,1,4,13.12),(3,6,1,1,4,13.12),(3,7,1,1,4,13.12),(3,8,1,1,4,13.12),(3,9,1,1,6,19.68),(6,2,1,1,4,13.12),(6,3,1,1,4,13.12),(6,4,1,1,4,13.12),(6,5,1,1,4,13.12),(6,6,1,1,4,13.12),(6,7,1,1,4,13.12),(6,8,1,1,4,13.12),(6,9,1,1,6,19.68),(7,5,2,1,4,13.12),(7,6,2,1,4,13.12),(7,7,2,1,4,13.12),(7,8,2,1,4,13.12),(7,9,2,1,6,19.68),(7,33,2,1,6,19.68),(8,9,2,2,6,19.68),(8,33,2,2,6,19.68),(7,5,2,2,4,13.12),(7,6,2,2,4,13.12),(7,7,2,2,4,13.12),(7,8,2,2,4,13.12),(7,9,2,2,6,19.68),(7,33,2,2,6,19.68),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11297,21 +11290,18 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H32" si="0">G3*3.28</f>
+        <f t="shared" ref="G3:G32" si="0">F3*3.28</f>
         <v>13.12</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I32" si="1">_xlfn.CONCAT( "(",B3,", ", C3,", ", D3,", ", E3,", ", F3,", ", G3,", ", H3,")")</f>
-        <v>(3, 2, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT( "(",B3,",", C3,",", D3,",", E3,",", F3,",", G3,")")</f>
+        <v>(3,2,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11328,21 +11318,18 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="1"/>
-        <v>(3, 3, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f>_xlfn.CONCAT( "(",B4,",", C4,",", D4,",", E4,",", F4,",", G4,")")</f>
+        <v>(3,3,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11359,21 +11346,18 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="1"/>
-        <v>(3, 4, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f>_xlfn.CONCAT( "(",B5,",", C5,",", D5,",", E5,",", F5,",", G5,")")</f>
+        <v>(3,4,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11390,21 +11374,18 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="1"/>
-        <v>(3, 5, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f>_xlfn.CONCAT( "(",B6,",", C6,",", D6,",", E6,",", F6,",", G6,")")</f>
+        <v>(3,5,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11421,21 +11402,18 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="1"/>
-        <v>(3, 6, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" t="str">
+        <f>_xlfn.CONCAT( "(",B7,",", C7,",", D7,",", E7,",", F7,",", G7,")")</f>
+        <v>(3,6,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11452,21 +11430,18 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="1"/>
-        <v>(3, 7, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" t="str">
+        <f>_xlfn.CONCAT( "(",B8,",", C8,",", D8,",", E8,",", F8,",", G8,")")</f>
+        <v>(3,7,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11483,21 +11458,18 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="1"/>
-        <v>(3, 8, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H9" t="str">
+        <f>_xlfn.CONCAT( "(",B9,",", C9,",", D9,",", E9,",", F9,",", G9,")")</f>
+        <v>(3,8,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11514,21 +11486,18 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G10">
-        <v>6</v>
-      </c>
-      <c r="H10">
         <f t="shared" si="0"/>
         <v>19.68</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="1"/>
-        <v>(3, 9, 1, 1, 1, 6, 19.68)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10" t="str">
+        <f>_xlfn.CONCAT( "(",B10,",", C10,",", D10,",", E10,",", F10,",", G10,")")</f>
+        <v>(3,9,1,1,6,19.68)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11545,21 +11514,18 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="1"/>
-        <v>(6, 2, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" t="str">
+        <f>_xlfn.CONCAT( "(",B11,",", C11,",", D11,",", E11,",", F11,",", G11,")")</f>
+        <v>(6,2,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11576,21 +11542,18 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="1"/>
-        <v>(6, 3, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <f>_xlfn.CONCAT( "(",B12,",", C12,",", D12,",", E12,",", F12,",", G12,")")</f>
+        <v>(6,3,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11607,21 +11570,18 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="H13">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="1"/>
-        <v>(6, 4, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" t="str">
+        <f>_xlfn.CONCAT( "(",B13,",", C13,",", D13,",", E13,",", F13,",", G13,")")</f>
+        <v>(6,4,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11638,21 +11598,18 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="1"/>
-        <v>(6, 5, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" t="str">
+        <f>_xlfn.CONCAT( "(",B14,",", C14,",", D14,",", E14,",", F14,",", G14,")")</f>
+        <v>(6,5,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11669,21 +11626,18 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>4</v>
-      </c>
-      <c r="H15">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="1"/>
-        <v>(6, 6, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" t="str">
+        <f>_xlfn.CONCAT( "(",B15,",", C15,",", D15,",", E15,",", F15,",", G15,")")</f>
+        <v>(6,6,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11700,21 +11654,18 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="H16">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="1"/>
-        <v>(6, 7, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" t="str">
+        <f>_xlfn.CONCAT( "(",B16,",", C16,",", D16,",", E16,",", F16,",", G16,")")</f>
+        <v>(6,7,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11731,21 +11682,18 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G17">
-        <v>4</v>
-      </c>
-      <c r="H17">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="1"/>
-        <v>(6, 8, 1, 1, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" t="str">
+        <f>_xlfn.CONCAT( "(",B17,",", C17,",", D17,",", E17,",", F17,",", G17,")")</f>
+        <v>(6,8,1,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11762,21 +11710,18 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G18">
-        <v>6</v>
-      </c>
-      <c r="H18">
         <f t="shared" si="0"/>
         <v>19.68</v>
       </c>
-      <c r="I18" t="str">
-        <f t="shared" si="1"/>
-        <v>(6, 9, 1, 1, 1, 6, 19.68)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" t="str">
+        <f>_xlfn.CONCAT( "(",B18,",", C18,",", D18,",", E18,",", F18,",", G18,")")</f>
+        <v>(6,9,1,1,6,19.68)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11787,27 +11732,24 @@
         <v>5</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G19">
-        <v>4</v>
-      </c>
-      <c r="H19">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I19" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 5, 1, 2, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" t="str">
+        <f>_xlfn.CONCAT( "(",B19,",", C19,",", D19,",", E19,",", F19,",", G19,")")</f>
+        <v>(7,5,2,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11818,27 +11760,24 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G20">
-        <v>4</v>
-      </c>
-      <c r="H20">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I20" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 6, 1, 2, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" t="str">
+        <f>_xlfn.CONCAT( "(",B20,",", C20,",", D20,",", E20,",", F20,",", G20,")")</f>
+        <v>(7,6,2,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -11849,27 +11788,24 @@
         <v>7</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G21">
-        <v>4</v>
-      </c>
-      <c r="H21">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 7, 1, 2, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" t="str">
+        <f>_xlfn.CONCAT( "(",B21,",", C21,",", D21,",", E21,",", F21,",", G21,")")</f>
+        <v>(7,7,2,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -11880,27 +11816,24 @@
         <v>8</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G22">
-        <v>4</v>
-      </c>
-      <c r="H22">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I22" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 8, 1, 2, 1, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" t="str">
+        <f>_xlfn.CONCAT( "(",B22,",", C22,",", D22,",", E22,",", F22,",", G22,")")</f>
+        <v>(7,8,2,1,4,13.12)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -11911,27 +11844,24 @@
         <v>9</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G23">
-        <v>6</v>
-      </c>
-      <c r="H23">
         <f t="shared" si="0"/>
         <v>19.68</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 9, 1, 2, 1, 6, 19.68)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" t="str">
+        <f>_xlfn.CONCAT( "(",B23,",", C23,",", D23,",", E23,",", F23,",", G23,")")</f>
+        <v>(7,9,2,1,6,19.68)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -11942,27 +11872,24 @@
         <v>33</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G24">
-        <v>6</v>
-      </c>
-      <c r="H24">
         <f t="shared" si="0"/>
         <v>19.68</v>
       </c>
-      <c r="I24" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 33, 1, 2, 1, 6, 19.68)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" t="str">
+        <f>_xlfn.CONCAT( "(",B24,",", C24,",", D24,",", E24,",", F24,",", G24,")")</f>
+        <v>(7,33,2,1,6,19.68)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -11973,27 +11900,24 @@
         <v>9</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>2</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>6</v>
-      </c>
-      <c r="H25">
         <f t="shared" si="0"/>
         <v>19.68</v>
       </c>
-      <c r="I25" t="str">
-        <f t="shared" si="1"/>
-        <v>(8, 9, 1, 2, 2, 6, 19.68)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" t="str">
+        <f>_xlfn.CONCAT( "(",B25,",", C25,",", D25,",", E25,",", F25,",", G25,")")</f>
+        <v>(8,9,2,2,6,19.68)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -12004,27 +11928,24 @@
         <v>33</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G26">
-        <v>6</v>
-      </c>
-      <c r="H26">
         <f t="shared" si="0"/>
         <v>19.68</v>
       </c>
-      <c r="I26" t="str">
-        <f t="shared" si="1"/>
-        <v>(8, 33, 1, 2, 2, 6, 19.68)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" t="str">
+        <f>_xlfn.CONCAT( "(",B26,",", C26,",", D26,",", E26,",", F26,",", G26,")")</f>
+        <v>(8,33,2,2,6,19.68)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -12035,27 +11956,24 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G27">
-        <v>4</v>
-      </c>
-      <c r="H27">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I27" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 5, 1, 2, 2, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" t="str">
+        <f>_xlfn.CONCAT( "(",B27,",", C27,",", D27,",", E27,",", F27,",", G27,")")</f>
+        <v>(7,5,2,2,4,13.12)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -12066,27 +11984,24 @@
         <v>6</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G28">
-        <v>4</v>
-      </c>
-      <c r="H28">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I28" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 6, 1, 2, 2, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <f>_xlfn.CONCAT( "(",B28,",", C28,",", D28,",", E28,",", F28,",", G28,")")</f>
+        <v>(7,6,2,2,4,13.12)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -12097,27 +12012,24 @@
         <v>7</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
         <v>2</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G29">
-        <v>4</v>
-      </c>
-      <c r="H29">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I29" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 7, 1, 2, 2, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <f>_xlfn.CONCAT( "(",B29,",", C29,",", D29,",", E29,",", F29,",", G29,")")</f>
+        <v>(7,7,2,2,4,13.12)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -12128,27 +12040,24 @@
         <v>8</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G30">
-        <v>4</v>
-      </c>
-      <c r="H30">
         <f t="shared" si="0"/>
         <v>13.12</v>
       </c>
-      <c r="I30" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 8, 1, 2, 2, 4, 13.12)</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" t="str">
+        <f>_xlfn.CONCAT( "(",B30,",", C30,",", D30,",", E30,",", F30,",", G30,")")</f>
+        <v>(7,8,2,2,4,13.12)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -12159,27 +12068,24 @@
         <v>9</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G31">
-        <v>6</v>
-      </c>
-      <c r="H31">
         <f t="shared" si="0"/>
         <v>19.68</v>
       </c>
-      <c r="I31" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 9, 1, 2, 2, 6, 19.68)</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <f>_xlfn.CONCAT( "(",B31,",", C31,",", D31,",", E31,",", F31,",", G31,")")</f>
+        <v>(7,9,2,2,6,19.68)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -12190,24 +12096,21 @@
         <v>33</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32">
         <v>2</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G32">
-        <v>6</v>
-      </c>
-      <c r="H32">
         <f t="shared" si="0"/>
         <v>19.68</v>
       </c>
-      <c r="I32" t="str">
-        <f t="shared" si="1"/>
-        <v>(7, 33, 1, 2, 2, 6, 19.68)</v>
+      <c r="H32" t="str">
+        <f>_xlfn.CONCAT( "(",B32,",", C32,",", D32,",", E32,",", F32,",", G32,")")</f>
+        <v>(7,33,2,2,6,19.68)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>